<commit_message>
Debugging naive component forecast
</commit_message>
<xml_diff>
--- a/0_1_Output_Data/2_YoY_Forecast_Vectors/forecast_series_yoy_AVERAGE_10_9_full.xlsx
+++ b/0_1_Output_Data/2_YoY_Forecast_Vectors/forecast_series_yoy_AVERAGE_10_9_full.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfbe04e23282f0d1/Desktop/ifo/Konjunkturprognose Evaluierung/ifo Forecast Evaluation Workfolder/0_1_Output_Data/2_YoY_Forecast_Vectors/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_CA84C7309E01513894FE31D2F87AE3807806190C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56274871-A7BD-4744-AD68-36C720AD9171}"/>
   <bookViews>
-    <workbookView xWindow="9010" yWindow="5450" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -40,11 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,25 +100,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -162,7 +148,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -196,7 +182,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -231,10 +216,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -407,19 +391,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.08984375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -436,7 +415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>32508</v>
       </c>
@@ -444,16 +423,16 @@
         <v>1988</v>
       </c>
       <c r="C2">
-        <v>3.3099646074777671</v>
+        <v>3.309964607477767</v>
       </c>
       <c r="D2">
         <v>1989</v>
       </c>
       <c r="E2">
-        <v>3.2920793873987049</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.292079387398705</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>32598</v>
       </c>
@@ -461,16 +440,16 @@
         <v>1989</v>
       </c>
       <c r="C3">
-        <v>3.6884011156645968</v>
+        <v>3.688401115664597</v>
       </c>
       <c r="D3">
         <v>1990</v>
       </c>
       <c r="E3">
-        <v>2.8205363172195459</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.820536317219546</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>32689</v>
       </c>
@@ -478,7 +457,7 @@
         <v>1989</v>
       </c>
       <c r="C4">
-        <v>4.0708104987877034</v>
+        <v>4.070810498787703</v>
       </c>
       <c r="D4">
         <v>1990</v>
@@ -487,7 +466,7 @@
         <v>2.938039590662322</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>32781</v>
       </c>
@@ -495,7 +474,7 @@
         <v>1989</v>
       </c>
       <c r="C5">
-        <v>3.7816745469521522</v>
+        <v>3.781674546952152</v>
       </c>
       <c r="D5">
         <v>1990</v>
@@ -504,7 +483,7 @@
         <v>2.637960524935878</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>32873</v>
       </c>
@@ -518,10 +497,10 @@
         <v>1990</v>
       </c>
       <c r="E6">
-        <v>3.8947664554024319</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.894766455402432</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>32963</v>
       </c>
@@ -529,16 +508,16 @@
         <v>1990</v>
       </c>
       <c r="C7">
-        <v>3.7425369129473252</v>
+        <v>3.742536912947325</v>
       </c>
       <c r="D7">
         <v>1991</v>
       </c>
       <c r="E7">
-        <v>3.6605893878241651</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.660589387824165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>33054</v>
       </c>
@@ -546,16 +525,16 @@
         <v>1990</v>
       </c>
       <c r="C8">
-        <v>5.1606933312428938</v>
+        <v>5.160693331242894</v>
       </c>
       <c r="D8">
         <v>1991</v>
       </c>
       <c r="E8">
-        <v>4.2217273334223426</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.221727333422343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>33146</v>
       </c>
@@ -563,16 +542,16 @@
         <v>1990</v>
       </c>
       <c r="C9">
-        <v>4.6400548686180043</v>
+        <v>4.640054868618004</v>
       </c>
       <c r="D9">
         <v>1991</v>
       </c>
       <c r="E9">
-        <v>3.6577423538160621</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.657742353816062</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>33238</v>
       </c>
@@ -580,16 +559,16 @@
         <v>1990</v>
       </c>
       <c r="C10">
-        <v>5.3379175837574788</v>
+        <v>5.337917583757479</v>
       </c>
       <c r="D10">
         <v>1991</v>
       </c>
       <c r="E10">
-        <v>5.2716247001149519</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.271624700114952</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="2">
         <v>33328</v>
       </c>
@@ -597,16 +576,16 @@
         <v>1991</v>
       </c>
       <c r="C11">
-        <v>5.6792191516375379</v>
+        <v>5.679219151637538</v>
       </c>
       <c r="D11">
         <v>1992</v>
       </c>
       <c r="E11">
-        <v>4.9930929454505169</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.993092945450517</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
         <v>33419</v>
       </c>
@@ -614,16 +593,16 @@
         <v>1991</v>
       </c>
       <c r="C12">
-        <v>7.5463669878942818</v>
+        <v>7.546366987894282</v>
       </c>
       <c r="D12">
         <v>1992</v>
       </c>
       <c r="E12">
-        <v>5.6834523227490941</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.683452322749094</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="2">
         <v>33511</v>
       </c>
@@ -631,16 +610,16 @@
         <v>1991</v>
       </c>
       <c r="C13">
-        <v>7.3167716210998268</v>
+        <v>7.316771621099827</v>
       </c>
       <c r="D13">
         <v>1992</v>
       </c>
       <c r="E13">
-        <v>5.5785362578704811</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.578536257870481</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="2">
         <v>33603</v>
       </c>
@@ -648,7 +627,7 @@
         <v>1991</v>
       </c>
       <c r="C14">
-        <v>6.2108503582882344</v>
+        <v>6.210850358288234</v>
       </c>
       <c r="D14">
         <v>1992</v>
@@ -657,7 +636,7 @@
         <v>4.003658823348033</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5">
       <c r="A15" s="2">
         <v>33694</v>
       </c>
@@ -674,7 +653,7 @@
         <v>5.161383041660117</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5">
       <c r="A16" s="2">
         <v>33785</v>
       </c>
@@ -682,16 +661,16 @@
         <v>1992</v>
       </c>
       <c r="C16">
-        <v>4.0062453214550384</v>
+        <v>4.006245321455038</v>
       </c>
       <c r="D16">
         <v>1993</v>
       </c>
       <c r="E16">
-        <v>5.3477023298620363</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.347702329862036</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>33877</v>
       </c>
@@ -699,16 +678,16 @@
         <v>1992</v>
       </c>
       <c r="C17">
-        <v>2.8647569961665291</v>
+        <v>2.864756996166529</v>
       </c>
       <c r="D17">
         <v>1993</v>
       </c>
       <c r="E17">
-        <v>4.5270615394133573</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.527061539413357</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
         <v>33969</v>
       </c>
@@ -716,16 +695,16 @@
         <v>1992</v>
       </c>
       <c r="C18">
-        <v>2.1208967418604452</v>
+        <v>2.120896741860445</v>
       </c>
       <c r="D18">
         <v>1993</v>
       </c>
       <c r="E18">
-        <v>3.0935187936087289</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.093518793608729</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
         <v>34059</v>
       </c>
@@ -733,7 +712,7 @@
         <v>1993</v>
       </c>
       <c r="C19">
-        <v>2.0889766925624942</v>
+        <v>2.088976692562494</v>
       </c>
       <c r="D19">
         <v>1994</v>
@@ -742,7 +721,7 @@
         <v>3.668026874948116</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5">
       <c r="A20" s="2">
         <v>34150</v>
       </c>
@@ -756,10 +735,10 @@
         <v>1994</v>
       </c>
       <c r="E20">
-        <v>2.0739015570438109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.073901557043811</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="2">
         <v>34242</v>
       </c>
@@ -767,7 +746,7 @@
         <v>1993</v>
       </c>
       <c r="C21">
-        <v>-1.2147343529862691</v>
+        <v>-1.214734352986269</v>
       </c>
       <c r="D21">
         <v>1994</v>
@@ -776,7 +755,7 @@
         <v>1.668515919881242</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5">
       <c r="A22" s="2">
         <v>34334</v>
       </c>
@@ -784,16 +763,16 @@
         <v>1993</v>
       </c>
       <c r="C22">
-        <v>-1.1051511183786671</v>
+        <v>-1.105151118378667</v>
       </c>
       <c r="D22">
         <v>1994</v>
       </c>
       <c r="E22">
-        <v>1.1621462624355821</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.162146262435582</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="2">
         <v>34424</v>
       </c>
@@ -801,16 +780,16 @@
         <v>1994</v>
       </c>
       <c r="C23">
-        <v>0.53799661760194351</v>
+        <v>0.5379966176019435</v>
       </c>
       <c r="D23">
         <v>1995</v>
       </c>
       <c r="E23">
-        <v>0.26472991975321492</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.2647299197532149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="2">
         <v>34515</v>
       </c>
@@ -824,10 +803,10 @@
         <v>1995</v>
       </c>
       <c r="E24">
-        <v>0.97887306378079408</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.9788730637807941</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="2">
         <v>34607</v>
       </c>
@@ -835,7 +814,7 @@
         <v>1994</v>
       </c>
       <c r="C25">
-        <v>2.7087871264884988</v>
+        <v>2.708787126488499</v>
       </c>
       <c r="D25">
         <v>1995</v>
@@ -844,7 +823,7 @@
         <v>1.362511602832805</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5">
       <c r="A26" s="2">
         <v>34699</v>
       </c>
@@ -852,16 +831,16 @@
         <v>1994</v>
       </c>
       <c r="C26">
-        <v>2.8660960897735288</v>
+        <v>2.866096089773529</v>
       </c>
       <c r="D26">
         <v>1995</v>
       </c>
       <c r="E26">
-        <v>1.2952743499062389</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.295274349906239</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="2">
         <v>34789</v>
       </c>
@@ -869,7 +848,7 @@
         <v>1995</v>
       </c>
       <c r="C27">
-        <v>1.7731434398668531</v>
+        <v>1.773143439866853</v>
       </c>
       <c r="D27">
         <v>1996</v>
@@ -878,7 +857,7 @@
         <v>1.098119484585292</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5">
       <c r="A28" s="2">
         <v>34880</v>
       </c>
@@ -892,10 +871,10 @@
         <v>1996</v>
       </c>
       <c r="E28">
-        <v>1.2452938179490669</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.245293817949067</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="2">
         <v>34948</v>
       </c>
@@ -903,16 +882,16 @@
         <v>1995</v>
       </c>
       <c r="C29">
-        <v>2.4375372545399898</v>
+        <v>2.43753725453999</v>
       </c>
       <c r="D29">
         <v>1996</v>
       </c>
       <c r="E29">
-        <v>1.8915819972123991</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.891581997212399</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="2">
         <v>35040</v>
       </c>
@@ -929,7 +908,7 @@
         <v>2.253863008704204</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5">
       <c r="A31" s="2">
         <v>35131</v>
       </c>
@@ -943,10 +922,10 @@
         <v>1997</v>
       </c>
       <c r="E31">
-        <v>2.1010217825220501</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.10102178252205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="2">
         <v>35221</v>
       </c>
@@ -954,16 +933,16 @@
         <v>1996</v>
       </c>
       <c r="C32">
-        <v>0.39646863237294833</v>
+        <v>0.3964686323729483</v>
       </c>
       <c r="D32">
         <v>1997</v>
       </c>
       <c r="E32">
-        <v>1.7379451715984651</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.737945171598465</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="2">
         <v>35313</v>
       </c>
@@ -971,16 +950,16 @@
         <v>1996</v>
       </c>
       <c r="C33">
-        <v>1.2933308149846829</v>
+        <v>1.293330814984683</v>
       </c>
       <c r="D33">
         <v>1997</v>
       </c>
       <c r="E33">
-        <v>2.5133400504567138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.513340050456714</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="2">
         <v>35403</v>
       </c>
@@ -988,16 +967,16 @@
         <v>1996</v>
       </c>
       <c r="C34">
-        <v>1.4408272659405921</v>
+        <v>1.440827265940592</v>
       </c>
       <c r="D34">
         <v>1997</v>
       </c>
       <c r="E34">
-        <v>2.5078611613149842</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.507861161314984</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="2">
         <v>35493</v>
       </c>
@@ -1005,16 +984,16 @@
         <v>1997</v>
       </c>
       <c r="C35">
-        <v>1.9420930280907409</v>
+        <v>1.942093028090741</v>
       </c>
       <c r="D35">
         <v>1998</v>
       </c>
       <c r="E35">
-        <v>1.8176933497203951</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.817693349720395</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="2">
         <v>35586</v>
       </c>
@@ -1022,16 +1001,16 @@
         <v>1997</v>
       </c>
       <c r="C36">
-        <v>1.9112291760793321</v>
+        <v>1.911229176079332</v>
       </c>
       <c r="D36">
         <v>1998</v>
       </c>
       <c r="E36">
-        <v>1.7655742137510311</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.765574213751031</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="2">
         <v>35683</v>
       </c>
@@ -1045,10 +1024,10 @@
         <v>1998</v>
       </c>
       <c r="E37">
-        <v>1.8133364642780809</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.813336464278081</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="2">
         <v>35768</v>
       </c>
@@ -1056,7 +1035,7 @@
         <v>1997</v>
       </c>
       <c r="C38">
-        <v>2.3887900183338528</v>
+        <v>2.388790018333853</v>
       </c>
       <c r="D38">
         <v>1998</v>
@@ -1065,7 +1044,7 @@
         <v>2.172278666428507</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5">
       <c r="A39" s="2">
         <v>35881</v>
       </c>
@@ -1079,10 +1058,10 @@
         <v>1999</v>
       </c>
       <c r="E39">
-        <v>1.6829431222661779</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.682943122266178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="2">
         <v>35950</v>
       </c>
@@ -1090,16 +1069,16 @@
         <v>1998</v>
       </c>
       <c r="C40">
-        <v>2.6043013169259281</v>
+        <v>2.604301316925928</v>
       </c>
       <c r="D40">
         <v>1999</v>
       </c>
       <c r="E40">
-        <v>2.1712226077138741</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.171222607713874</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="2">
         <v>36047</v>
       </c>
@@ -1107,7 +1086,7 @@
         <v>1998</v>
       </c>
       <c r="C41">
-        <v>2.7585961889704969</v>
+        <v>2.758596188970497</v>
       </c>
       <c r="D41">
         <v>1999</v>
@@ -1116,7 +1095,7 @@
         <v>2.26748870303155</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5">
       <c r="A42" s="2">
         <v>36132</v>
       </c>
@@ -1130,10 +1109,10 @@
         <v>1999</v>
       </c>
       <c r="E42">
-        <v>2.6497789012486672</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.649778901248667</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="2">
         <v>36223</v>
       </c>
@@ -1147,10 +1126,10 @@
         <v>2000</v>
       </c>
       <c r="E43">
-        <v>1.9933165185815671</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.993316518581567</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="2">
         <v>36319</v>
       </c>
@@ -1158,16 +1137,16 @@
         <v>1999</v>
       </c>
       <c r="C44">
-        <v>1.1583241735758421</v>
+        <v>1.158324173575842</v>
       </c>
       <c r="D44">
         <v>2000</v>
       </c>
       <c r="E44">
-        <v>1.5829236631093699</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.58292366310937</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="2">
         <v>36412</v>
       </c>
@@ -1175,7 +1154,7 @@
         <v>1999</v>
       </c>
       <c r="C45">
-        <v>0.71695109292988501</v>
+        <v>0.716951092929885</v>
       </c>
       <c r="D45">
         <v>2000</v>
@@ -1184,7 +1163,7 @@
         <v>1.183079735375214</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5">
       <c r="A46" s="2">
         <v>36501</v>
       </c>
@@ -1201,7 +1180,7 @@
         <v>1.878782575038151</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5">
       <c r="A47" s="2">
         <v>36587</v>
       </c>
@@ -1218,7 +1197,7 @@
         <v>1.70996454095349</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5">
       <c r="A48" s="2">
         <v>36676</v>
       </c>
@@ -1235,7 +1214,7 @@
         <v>1.845439021891959</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5">
       <c r="A49" s="2">
         <v>36767</v>
       </c>
@@ -1243,7 +1222,7 @@
         <v>2000</v>
       </c>
       <c r="C49">
-        <v>3.0392479947094491</v>
+        <v>3.039247994709449</v>
       </c>
       <c r="D49">
         <v>2001</v>
@@ -1252,7 +1231,7 @@
         <v>2.286406977081445</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5">
       <c r="A50" s="2">
         <v>36858</v>
       </c>
@@ -1266,10 +1245,10 @@
         <v>2001</v>
       </c>
       <c r="E50">
-        <v>2.1414130021199411</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.141413002119941</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="2">
         <v>36951</v>
       </c>
@@ -1277,16 +1256,16 @@
         <v>2001</v>
       </c>
       <c r="C51">
-        <v>1.9472783437670891</v>
+        <v>1.947278343767089</v>
       </c>
       <c r="D51">
         <v>2002</v>
       </c>
       <c r="E51">
-        <v>2.1664359589748772</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.166435958974877</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="2">
         <v>37034</v>
       </c>
@@ -1294,7 +1273,7 @@
         <v>2001</v>
       </c>
       <c r="C52">
-        <v>1.7896540242653189</v>
+        <v>1.789654024265319</v>
       </c>
       <c r="D52">
         <v>2002</v>
@@ -1303,7 +1282,7 @@
         <v>2.196383146547265</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5">
       <c r="A53" s="2">
         <v>37126</v>
       </c>
@@ -1311,16 +1290,16 @@
         <v>2001</v>
       </c>
       <c r="C53">
-        <v>1.2867241925820889</v>
+        <v>1.286724192582089</v>
       </c>
       <c r="D53">
         <v>2002</v>
       </c>
       <c r="E53">
-        <v>2.2017876090316908</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.201787609031691</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="2">
         <v>37222</v>
       </c>
@@ -1328,7 +1307,7 @@
         <v>2001</v>
       </c>
       <c r="C54">
-        <v>0.88811970530715545</v>
+        <v>0.8881197053071554</v>
       </c>
       <c r="D54">
         <v>2002</v>
@@ -1337,7 +1316,7 @@
         <v>1.417229954124744</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5">
       <c r="A55" s="2">
         <v>37314</v>
       </c>
@@ -1345,16 +1324,16 @@
         <v>2002</v>
       </c>
       <c r="C55">
-        <v>0.88217760257651712</v>
+        <v>0.8821776025765171</v>
       </c>
       <c r="D55">
         <v>2003</v>
       </c>
       <c r="E55">
-        <v>1.8417933279397001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.8417933279397</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="2">
         <v>37399</v>
       </c>
@@ -1362,7 +1341,7 @@
         <v>2002</v>
       </c>
       <c r="C56">
-        <v>0.43003987040877162</v>
+        <v>0.4300398704087716</v>
       </c>
       <c r="D56">
         <v>2003</v>
@@ -1371,7 +1350,7 @@
         <v>1.402332333946066</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5">
       <c r="A57" s="2">
         <v>37490</v>
       </c>
@@ -1379,7 +1358,7 @@
         <v>2002</v>
       </c>
       <c r="C57">
-        <v>0.34986649440604811</v>
+        <v>0.3498664944060481</v>
       </c>
       <c r="D57">
         <v>2003</v>
@@ -1388,7 +1367,7 @@
         <v>1.029333720985703</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5">
       <c r="A58" s="2">
         <v>37581</v>
       </c>
@@ -1402,10 +1381,10 @@
         <v>2003</v>
       </c>
       <c r="E58">
-        <v>0.81146233729509909</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.8114623372950991</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="2">
         <v>37678</v>
       </c>
@@ -1413,16 +1392,16 @@
         <v>2003</v>
       </c>
       <c r="C59">
-        <v>0.39550676201871582</v>
+        <v>0.3955067620187158</v>
       </c>
       <c r="D59">
         <v>2004</v>
       </c>
       <c r="E59">
-        <v>0.36595034947133342</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.3659503494713334</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="2">
         <v>37756</v>
       </c>
@@ -1430,7 +1409,7 @@
         <v>2003</v>
       </c>
       <c r="C60">
-        <v>3.5111677398425023E-2</v>
+        <v>0.03511167739842502</v>
       </c>
       <c r="D60">
         <v>2004</v>
@@ -1439,7 +1418,7 @@
         <v>0.2562430727641285</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5">
       <c r="A61" s="2">
         <v>37847</v>
       </c>
@@ -1453,10 +1432,10 @@
         <v>2004</v>
       </c>
       <c r="E61">
-        <v>0.25972329491874557</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.2597232949187456</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" s="2">
         <v>37938</v>
       </c>
@@ -1464,16 +1443,16 @@
         <v>2003</v>
       </c>
       <c r="C62">
-        <v>-0.16059721877719199</v>
+        <v>-0.160597218777192</v>
       </c>
       <c r="D62">
         <v>2004</v>
       </c>
       <c r="E62">
-        <v>6.8663074916619493E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.06866307491661949</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" s="2">
         <v>38029</v>
       </c>
@@ -1487,10 +1466,10 @@
         <v>2005</v>
       </c>
       <c r="E63">
-        <v>8.4971346270057424E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.08497134627005742</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" s="2">
         <v>38120</v>
       </c>
@@ -1498,16 +1477,16 @@
         <v>2004</v>
       </c>
       <c r="C64">
-        <v>0.82783622397992751</v>
+        <v>0.8278362239799275</v>
       </c>
       <c r="D64">
         <v>2005</v>
       </c>
       <c r="E64">
-        <v>0.33901773885884889</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.3390177388588489</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" s="2">
         <v>38211</v>
       </c>
@@ -1515,16 +1494,16 @@
         <v>2004</v>
       </c>
       <c r="C65">
-        <v>1.2097019687231649</v>
+        <v>1.209701968723165</v>
       </c>
       <c r="D65">
         <v>2005</v>
       </c>
       <c r="E65">
-        <v>0.64494757520729973</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.6449475752072997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" s="2">
         <v>38302</v>
       </c>
@@ -1532,16 +1511,16 @@
         <v>2004</v>
       </c>
       <c r="C66">
-        <v>1.1424219572799821</v>
+        <v>1.142421957279982</v>
       </c>
       <c r="D66">
         <v>2005</v>
       </c>
       <c r="E66">
-        <v>0.61025477079812429</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.6102547707981243</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" s="2">
         <v>38398</v>
       </c>
@@ -1549,16 +1528,16 @@
         <v>2005</v>
       </c>
       <c r="C67">
-        <v>0.14866779743334391</v>
+        <v>0.1486677974333439</v>
       </c>
       <c r="D67">
         <v>2006</v>
       </c>
       <c r="E67">
-        <v>0.35942199116503198</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.359421991165032</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" s="2">
         <v>38484</v>
       </c>
@@ -1575,7 +1554,7 @@
         <v>0.667546990777379</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5">
       <c r="A69" s="2">
         <v>38575</v>
       </c>
@@ -1589,10 +1568,10 @@
         <v>2006</v>
       </c>
       <c r="E69">
-        <v>0.52672089814400636</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.5267208981440064</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" s="2">
         <v>38671</v>
       </c>
@@ -1609,7 +1588,7 @@
         <v>1.236500865721557</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5">
       <c r="A71" s="2">
         <v>38762</v>
       </c>
@@ -1626,7 +1605,7 @@
         <v>1.176263924936682</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5">
       <c r="A72" s="2">
         <v>38848</v>
       </c>
@@ -1640,10 +1619,10 @@
         <v>2007</v>
       </c>
       <c r="E72">
-        <v>1.2345897502288981</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.234589750228898</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="2">
         <v>38943</v>
       </c>
@@ -1651,7 +1630,7 @@
         <v>2006</v>
       </c>
       <c r="C73">
-        <v>2.1525281476818758</v>
+        <v>2.152528147681876</v>
       </c>
       <c r="D73">
         <v>2007</v>
@@ -1660,7 +1639,7 @@
         <v>1.519596551719538</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5">
       <c r="A74" s="2">
         <v>39035</v>
       </c>
@@ -1668,16 +1647,16 @@
         <v>2006</v>
       </c>
       <c r="C74">
-        <v>2.5739993744375189</v>
+        <v>2.573999374437519</v>
       </c>
       <c r="D74">
         <v>2007</v>
       </c>
       <c r="E74">
-        <v>1.8894463395620289</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.889446339562029</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" s="2">
         <v>39126</v>
       </c>
@@ -1685,7 +1664,7 @@
         <v>2007</v>
       </c>
       <c r="C75">
-        <v>2.6771337632869319</v>
+        <v>2.677133763286932</v>
       </c>
       <c r="D75">
         <v>2008</v>
@@ -1694,7 +1673,7 @@
         <v>2.118492300568509</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5">
       <c r="A76" s="2">
         <v>39217</v>
       </c>
@@ -1708,10 +1687,10 @@
         <v>2008</v>
       </c>
       <c r="E76">
-        <v>2.4701142029330381</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.470114202933038</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" s="2">
         <v>39308</v>
       </c>
@@ -1719,7 +1698,7 @@
         <v>2007</v>
       </c>
       <c r="C77">
-        <v>2.6652472783111669</v>
+        <v>2.665247278311167</v>
       </c>
       <c r="D77">
         <v>2008</v>
@@ -1728,7 +1707,7 @@
         <v>2.448133414186437</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5">
       <c r="A78" s="2">
         <v>39400</v>
       </c>
@@ -1736,16 +1715,16 @@
         <v>2007</v>
       </c>
       <c r="C78">
-        <v>2.7014156853015341</v>
+        <v>2.701415685301534</v>
       </c>
       <c r="D78">
         <v>2008</v>
       </c>
       <c r="E78">
-        <v>2.5847365389251702</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.58473653892517</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" s="2">
         <v>39492</v>
       </c>
@@ -1759,10 +1738,10 @@
         <v>2009</v>
       </c>
       <c r="E79">
-        <v>2.6171850790328581</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.617185079032858</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" s="2">
         <v>39583</v>
       </c>
@@ -1776,10 +1755,10 @@
         <v>2009</v>
       </c>
       <c r="E80">
-        <v>3.0100644400804288</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.010064440080429</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="2">
         <v>39674</v>
       </c>
@@ -1787,16 +1766,16 @@
         <v>2008</v>
       </c>
       <c r="C81">
-        <v>2.0378956459346842</v>
+        <v>2.037895645934684</v>
       </c>
       <c r="D81">
         <v>2009</v>
       </c>
       <c r="E81">
-        <v>2.3520176571616869</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.352017657161687</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" s="2">
         <v>39765</v>
       </c>
@@ -1810,10 +1789,10 @@
         <v>2009</v>
       </c>
       <c r="E82">
-        <v>1.3867257025007129</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.386725702500713</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" s="2">
         <v>39857</v>
       </c>
@@ -1821,16 +1800,16 @@
         <v>2009</v>
       </c>
       <c r="C83">
-        <v>-1.5368906529256381</v>
+        <v>-1.536890652925638</v>
       </c>
       <c r="D83">
         <v>2010</v>
       </c>
       <c r="E83">
-        <v>0.72930516826501535</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.7293051682650153</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" s="2">
         <v>39948</v>
       </c>
@@ -1838,16 +1817,16 @@
         <v>2009</v>
       </c>
       <c r="C84">
-        <v>-6.1894429607279644</v>
+        <v>-6.189442960727964</v>
       </c>
       <c r="D84">
         <v>2010</v>
       </c>
       <c r="E84">
-        <v>-1.1151795555465189</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+        <v>-1.115179555546519</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="2">
         <v>40038</v>
       </c>
@@ -1855,16 +1834,16 @@
         <v>2009</v>
       </c>
       <c r="C85">
-        <v>-5.6163796286003764</v>
+        <v>-5.616379628600376</v>
       </c>
       <c r="D85">
         <v>2010</v>
       </c>
       <c r="E85">
-        <v>-1.1804925296078681</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+        <v>-1.180492529607868</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" s="2">
         <v>40130</v>
       </c>
@@ -1872,16 +1851,16 @@
         <v>2009</v>
       </c>
       <c r="C86">
-        <v>-5.0112640539116127</v>
+        <v>-5.011264053911613</v>
       </c>
       <c r="D86">
         <v>2010</v>
       </c>
       <c r="E86">
-        <v>-0.45213967490790319</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+        <v>-0.4521396749079032</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" s="2">
         <v>40221</v>
       </c>
@@ -1898,7 +1877,7 @@
         <v>-1.250042014667974</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5">
       <c r="A88" s="2">
         <v>40310</v>
       </c>
@@ -1906,7 +1885,7 @@
         <v>2010</v>
       </c>
       <c r="C88">
-        <v>0.22701971473049201</v>
+        <v>0.227019714730492</v>
       </c>
       <c r="D88">
         <v>2011</v>
@@ -1915,7 +1894,7 @@
         <v>-1.435416797561895</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5">
       <c r="A89" s="2">
         <v>40403</v>
       </c>
@@ -1923,16 +1902,16 @@
         <v>2010</v>
       </c>
       <c r="C89">
-        <v>2.7282752698363439</v>
+        <v>2.728275269836344</v>
       </c>
       <c r="D89">
         <v>2011</v>
       </c>
       <c r="E89">
-        <v>6.1999917985633417E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.06199991798563342</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="2">
         <v>40494</v>
       </c>
@@ -1946,10 +1925,10 @@
         <v>2011</v>
       </c>
       <c r="E90">
-        <v>0.35651210957734492</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.3565121095773449</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" s="2">
         <v>40589</v>
       </c>
@@ -1963,10 +1942,10 @@
         <v>2012</v>
       </c>
       <c r="E91">
-        <v>-0.25963508506379179</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+        <v>-0.2596350850637918</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" s="2">
         <v>40676</v>
       </c>
@@ -1974,16 +1953,16 @@
         <v>2011</v>
       </c>
       <c r="C92">
-        <v>2.9019432789286088</v>
+        <v>2.901943278928609</v>
       </c>
       <c r="D92">
         <v>2012</v>
       </c>
       <c r="E92">
-        <v>0.52339021633454053</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.5233902163345405</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" s="2">
         <v>40771</v>
       </c>
@@ -1991,16 +1970,16 @@
         <v>2011</v>
       </c>
       <c r="C93">
-        <v>2.9231464718595608</v>
+        <v>2.923146471859561</v>
       </c>
       <c r="D93">
         <v>2012</v>
       </c>
       <c r="E93">
-        <v>1.1753648033898889</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.175364803389889</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" s="2">
         <v>40862</v>
       </c>
@@ -2008,16 +1987,16 @@
         <v>2011</v>
       </c>
       <c r="C94">
-        <v>3.2666135462440238</v>
+        <v>3.266613546244024</v>
       </c>
       <c r="D94">
         <v>2012</v>
       </c>
       <c r="E94">
-        <v>2.8570594676522449</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.857059467652245</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" s="2">
         <v>40954</v>
       </c>
@@ -2025,7 +2004,7 @@
         <v>2012</v>
       </c>
       <c r="C95">
-        <v>2.0576667250575609</v>
+        <v>2.057666725057561</v>
       </c>
       <c r="D95">
         <v>2013</v>
@@ -2034,7 +2013,7 @@
         <v>2.945937531474097</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5">
       <c r="A96" s="2">
         <v>41044</v>
       </c>
@@ -2042,16 +2021,16 @@
         <v>2012</v>
       </c>
       <c r="C96">
-        <v>1.7902744254709719</v>
+        <v>1.790274425470972</v>
       </c>
       <c r="D96">
         <v>2013</v>
       </c>
       <c r="E96">
-        <v>2.8222188691171102</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.82221886911711</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" s="2">
         <v>41135</v>
       </c>
@@ -2059,7 +2038,7 @@
         <v>2012</v>
       </c>
       <c r="C97">
-        <v>1.4106927584820459</v>
+        <v>1.410692758482046</v>
       </c>
       <c r="D97">
         <v>2013</v>
@@ -2068,7 +2047,7 @@
         <v>2.665591140370926</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5">
       <c r="A98" s="2">
         <v>41228</v>
       </c>
@@ -2082,10 +2061,10 @@
         <v>2013</v>
       </c>
       <c r="E98">
-        <v>2.2935137460632582</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.293513746063258</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" s="2">
         <v>41319</v>
       </c>
@@ -2102,7 +2081,7 @@
         <v>1.460307044206965</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5">
       <c r="A100" s="2">
         <v>41409</v>
       </c>
@@ -2110,16 +2089,16 @@
         <v>2013</v>
       </c>
       <c r="C100">
-        <v>0.12368625718974791</v>
+        <v>0.1236862571897479</v>
       </c>
       <c r="D100">
         <v>2014</v>
       </c>
       <c r="E100">
-        <v>1.1588340713951431</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.158834071395143</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" s="2">
         <v>41500</v>
       </c>
@@ -2127,7 +2106,7 @@
         <v>2013</v>
       </c>
       <c r="C101">
-        <v>0.51515692104104893</v>
+        <v>0.5151569210410489</v>
       </c>
       <c r="D101">
         <v>2014</v>
@@ -2136,7 +2115,7 @@
         <v>1.384145559863281</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5">
       <c r="A102" s="2">
         <v>41592</v>
       </c>
@@ -2144,7 +2123,7 @@
         <v>2013</v>
       </c>
       <c r="C102">
-        <v>0.48613023839625402</v>
+        <v>0.486130238396254</v>
       </c>
       <c r="D102">
         <v>2014</v>
@@ -2153,7 +2132,7 @@
         <v>0.9879154814133928</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5">
       <c r="A103" s="2">
         <v>41684</v>
       </c>
@@ -2161,16 +2140,16 @@
         <v>2014</v>
       </c>
       <c r="C103">
-        <v>1.2018888517177471</v>
+        <v>1.201888851717747</v>
       </c>
       <c r="D103">
         <v>2015</v>
       </c>
       <c r="E103">
-        <v>0.91275974742490718</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.9127597474249072</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" s="2">
         <v>41774</v>
       </c>
@@ -2187,7 +2166,7 @@
         <v>1.070117761036204</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5">
       <c r="A105" s="2">
         <v>41865</v>
       </c>
@@ -2195,16 +2174,16 @@
         <v>2014</v>
       </c>
       <c r="C105">
-        <v>1.3653683004142709</v>
+        <v>1.365368300414271</v>
       </c>
       <c r="D105">
         <v>2015</v>
       </c>
       <c r="E105">
-        <v>0.61719631396597308</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.6171963139659731</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" s="2">
         <v>41957</v>
       </c>
@@ -2212,7 +2191,7 @@
         <v>2014</v>
       </c>
       <c r="C106">
-        <v>1.4621129148316261</v>
+        <v>1.462112914831626</v>
       </c>
       <c r="D106">
         <v>2015</v>
@@ -2221,7 +2200,7 @@
         <v>0.5584147504514414</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5">
       <c r="A107" s="2">
         <v>42048</v>
       </c>
@@ -2229,16 +2208,16 @@
         <v>2015</v>
       </c>
       <c r="C107">
-        <v>1.1055948110870959</v>
+        <v>1.105594811087096</v>
       </c>
       <c r="D107">
         <v>2016</v>
       </c>
       <c r="E107">
-        <v>0.90796929257777048</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.9079692925777705</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" s="2">
         <v>42137</v>
       </c>
@@ -2255,7 +2234,7 @@
         <v>0.9828438564608355</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5">
       <c r="A109" s="2">
         <v>42230</v>
       </c>
@@ -2272,7 +2251,7 @@
         <v>1.459098717642338</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5">
       <c r="A110" s="2">
         <v>42321</v>
       </c>
@@ -2289,7 +2268,7 @@
         <v>1.630702503967973</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5">
       <c r="A111" s="2">
         <v>42412</v>
       </c>
@@ -2297,16 +2276,16 @@
         <v>2016</v>
       </c>
       <c r="C111">
-        <v>1.3195519047655151</v>
+        <v>1.319551904765515</v>
       </c>
       <c r="D111">
         <v>2017</v>
       </c>
       <c r="E111">
-        <v>1.4059416121636299</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.40594161216363</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112" s="2">
         <v>42503</v>
       </c>
@@ -2314,16 +2293,16 @@
         <v>2016</v>
       </c>
       <c r="C112">
-        <v>1.6827886300215369</v>
+        <v>1.682788630021537</v>
       </c>
       <c r="D112">
         <v>2017</v>
       </c>
       <c r="E112">
-        <v>1.5240797855039729</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.524079785503973</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" s="2">
         <v>42594</v>
       </c>
@@ -2331,7 +2310,7 @@
         <v>2016</v>
       </c>
       <c r="C113">
-        <v>1.8484909867468651</v>
+        <v>1.848490986746865</v>
       </c>
       <c r="D113">
         <v>2017</v>
@@ -2340,7 +2319,7 @@
         <v>1.602982755478233</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5">
       <c r="A114" s="2">
         <v>42689</v>
       </c>
@@ -2354,10 +2333,10 @@
         <v>2017</v>
       </c>
       <c r="E114">
-        <v>1.3655677390915779</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.365567739091578</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" s="2">
         <v>42780</v>
       </c>
@@ -2365,7 +2344,7 @@
         <v>2017</v>
       </c>
       <c r="C115">
-        <v>1.5412976132164189</v>
+        <v>1.541297613216419</v>
       </c>
       <c r="D115">
         <v>2018</v>
@@ -2374,7 +2353,7 @@
         <v>1.653904202057443</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5">
       <c r="A116" s="2">
         <v>42867</v>
       </c>
@@ -2391,7 +2370,7 @@
         <v>1.792179635996094</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5">
       <c r="A117" s="2">
         <v>42962</v>
       </c>
@@ -2399,16 +2378,16 @@
         <v>2017</v>
       </c>
       <c r="C117">
-        <v>2.1214465329965519</v>
+        <v>2.121446532996552</v>
       </c>
       <c r="D117">
         <v>2018</v>
       </c>
       <c r="E117">
-        <v>1.8457882668204031</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.845788266820403</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" s="2">
         <v>43053</v>
       </c>
@@ -2416,7 +2395,7 @@
         <v>2017</v>
       </c>
       <c r="C118">
-        <v>2.5327467436123019</v>
+        <v>2.532746743612302</v>
       </c>
       <c r="D118">
         <v>2018</v>
@@ -2425,7 +2404,7 @@
         <v>2.340401793803593</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5">
       <c r="A119" s="2">
         <v>43145</v>
       </c>
@@ -2433,16 +2412,16 @@
         <v>2018</v>
       </c>
       <c r="C119">
-        <v>2.3684750534270771</v>
+        <v>2.368475053427077</v>
       </c>
       <c r="D119">
         <v>2019</v>
       </c>
       <c r="E119">
-        <v>2.2059428972385891</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.205942897238589</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" s="2">
         <v>43235</v>
       </c>
@@ -2456,10 +2435,10 @@
         <v>2019</v>
       </c>
       <c r="E120">
-        <v>2.1954141569586532</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.195414156958653</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121" s="2">
         <v>43326</v>
       </c>
@@ -2473,10 +2452,10 @@
         <v>2019</v>
       </c>
       <c r="E121">
-        <v>2.1969204473961219</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.196920447396122</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122" s="2">
         <v>43418</v>
       </c>
@@ -2484,16 +2463,16 @@
         <v>2018</v>
       </c>
       <c r="C122">
-        <v>1.5506095984644701</v>
+        <v>1.55060959846447</v>
       </c>
       <c r="D122">
         <v>2019</v>
       </c>
       <c r="E122">
-        <v>1.4503399104985439</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.450339910498544</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123" s="2">
         <v>43510</v>
       </c>
@@ -2510,7 +2489,7 @@
         <v>1.601377435264961</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5">
       <c r="A124" s="2">
         <v>43600</v>
       </c>
@@ -2527,7 +2506,7 @@
         <v>1.7038902012801</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5">
       <c r="A125" s="2">
         <v>43691</v>
       </c>
@@ -2535,16 +2514,16 @@
         <v>2019</v>
       </c>
       <c r="C125">
-        <v>0.85080968093318443</v>
+        <v>0.8508096809331844</v>
       </c>
       <c r="D125">
         <v>2020</v>
       </c>
       <c r="E125">
-        <v>1.5934702463057391</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.593470246305739</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" s="2">
         <v>43783</v>
       </c>
@@ -2552,16 +2531,16 @@
         <v>2019</v>
       </c>
       <c r="C126">
-        <v>0.60573360562696799</v>
+        <v>0.605733605626968</v>
       </c>
       <c r="D126">
         <v>2020</v>
       </c>
       <c r="E126">
-        <v>0.98756219883060492</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.9875621988306049</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" s="2">
         <v>43875</v>
       </c>
@@ -2569,7 +2548,7 @@
         <v>2020</v>
       </c>
       <c r="C127">
-        <v>0.72931290670317228</v>
+        <v>0.7293129067031723</v>
       </c>
       <c r="D127">
         <v>2021</v>
@@ -2578,7 +2557,7 @@
         <v>1.074363095002373</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5">
       <c r="A128" s="2">
         <v>43966</v>
       </c>
@@ -2586,7 +2565,7 @@
         <v>2020</v>
       </c>
       <c r="C128">
-        <v>-2.2981605677551808</v>
+        <v>-2.298160567755181</v>
       </c>
       <c r="D128">
         <v>2021</v>
@@ -2595,7 +2574,7 @@
         <v>-0.189504292099274</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5">
       <c r="A129" s="2">
         <v>44068</v>
       </c>
@@ -2603,16 +2582,16 @@
         <v>2020</v>
       </c>
       <c r="C129">
-        <v>-9.8573760151454017</v>
+        <v>-9.857376015145402</v>
       </c>
       <c r="D129">
         <v>2021</v>
       </c>
       <c r="E129">
-        <v>-6.5999470552043364</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+        <v>-6.599947055204336</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" s="2">
         <v>44159</v>
       </c>
@@ -2620,16 +2599,16 @@
         <v>2020</v>
       </c>
       <c r="C130">
-        <v>-5.3931578551502426</v>
+        <v>-5.393157855150243</v>
       </c>
       <c r="D130">
         <v>2021</v>
       </c>
       <c r="E130">
-        <v>0.66144025217049762</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.6614402521704976</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131" s="2">
         <v>44251</v>
       </c>
@@ -2637,16 +2616,16 @@
         <v>2021</v>
       </c>
       <c r="C131">
-        <v>1.1057076940096611</v>
+        <v>1.105707694009661</v>
       </c>
       <c r="D131">
         <v>2022</v>
       </c>
       <c r="E131">
-        <v>-0.97159810352072107</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+        <v>-0.9715981035207211</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132" s="2">
         <v>44341</v>
       </c>
@@ -2654,7 +2633,7 @@
         <v>2021</v>
       </c>
       <c r="C132">
-        <v>-0.40976225836374391</v>
+        <v>-0.4097622583637439</v>
       </c>
       <c r="D132">
         <v>2022</v>
@@ -2663,7 +2642,7 @@
         <v>-1.402182612722491</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5">
       <c r="A133" s="2">
         <v>44432</v>
       </c>
@@ -2680,7 +2659,7 @@
         <v>-0.1384117278926178</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5">
       <c r="A134" s="2">
         <v>44525</v>
       </c>
@@ -2688,16 +2667,16 @@
         <v>2021</v>
       </c>
       <c r="C134">
-        <v>2.6588798897413608</v>
+        <v>2.658879889741361</v>
       </c>
       <c r="D134">
         <v>2022</v>
       </c>
       <c r="E134">
-        <v>1.2463390381634909</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.246339038163491</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" s="2">
         <v>44617</v>
       </c>
@@ -2711,10 +2690,10 @@
         <v>2023</v>
       </c>
       <c r="E135">
-        <v>7.0775556294799813E-2</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.07077555629479981</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" s="2">
         <v>44706</v>
       </c>
@@ -2728,10 +2707,10 @@
         <v>2023</v>
       </c>
       <c r="E136">
-        <v>5.4029527847276881E-4</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.0005402952784727688</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" s="2">
         <v>44798</v>
       </c>
@@ -2739,16 +2718,16 @@
         <v>2022</v>
       </c>
       <c r="C137">
-        <v>1.8238916324694989</v>
+        <v>1.823891632469499</v>
       </c>
       <c r="D137">
         <v>2023</v>
       </c>
       <c r="E137">
-        <v>0.36632097600839408</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.3663209760083941</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138" s="2">
         <v>44890</v>
       </c>
@@ -2765,7 +2744,7 @@
         <v>1.097222285099164</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5">
       <c r="A139" s="2">
         <v>44981</v>
       </c>
@@ -2773,16 +2752,16 @@
         <v>2023</v>
       </c>
       <c r="C139">
-        <v>2.9150432908299879</v>
+        <v>2.915043290829988</v>
       </c>
       <c r="D139">
         <v>2024</v>
       </c>
       <c r="E139">
-        <v>4.7994146561944451</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.799414656194445</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140" s="2">
         <v>45071</v>
       </c>
@@ -2796,10 +2775,10 @@
         <v>2024</v>
       </c>
       <c r="E140">
-        <v>0.94279509218528901</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.942795092185289</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141" s="2">
         <v>45163</v>
       </c>
@@ -2807,16 +2786,16 @@
         <v>2023</v>
       </c>
       <c r="C141">
-        <v>-5.7189361598353187E-2</v>
+        <v>-0.05718936159835319</v>
       </c>
       <c r="D141">
         <v>2024</v>
       </c>
       <c r="E141">
-        <v>0.90342163006871257</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.9034216300687126</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142" s="2">
         <v>45254</v>
       </c>
@@ -2824,7 +2803,7 @@
         <v>2023</v>
       </c>
       <c r="C142">
-        <v>-2.4541927130372621E-2</v>
+        <v>-0.02454192713037262</v>
       </c>
       <c r="D142">
         <v>2024</v>
@@ -2833,7 +2812,7 @@
         <v>1.192480395252127</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5">
       <c r="A143" s="2">
         <v>45345</v>
       </c>
@@ -2847,10 +2826,10 @@
         <v>2025</v>
       </c>
       <c r="E143">
-        <v>0.53576033948961044</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.5357603394896104</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144" s="2">
         <v>45436</v>
       </c>
@@ -2858,16 +2837,16 @@
         <v>2024</v>
       </c>
       <c r="C144">
-        <v>2.1361434735411858E-2</v>
+        <v>0.02136143473541186</v>
       </c>
       <c r="D144">
         <v>2025</v>
       </c>
       <c r="E144">
-        <v>0.35383095300103312</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.3538309530010331</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145" s="2">
         <v>45534</v>
       </c>
@@ -2875,16 +2854,16 @@
         <v>2024</v>
       </c>
       <c r="C145">
-        <v>-2.68205859629056E-2</v>
+        <v>-0.0268205859629056</v>
       </c>
       <c r="D145">
         <v>2025</v>
       </c>
       <c r="E145">
-        <v>6.3862404253911542E-2</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.06386240425391154</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146" s="2">
         <v>45618</v>
       </c>
@@ -2892,16 +2871,16 @@
         <v>2024</v>
       </c>
       <c r="C146">
-        <v>-0.15701762235937891</v>
+        <v>-0.1570176223593789</v>
       </c>
       <c r="D146">
         <v>2025</v>
       </c>
       <c r="E146">
-        <v>-4.5446249791425419E-2</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+        <v>-0.04544624979142542</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147" s="2">
         <v>45713</v>
       </c>
@@ -2918,7 +2897,7 @@
         <v>-0.1049893300193228</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5">
       <c r="A148" s="2">
         <v>45800</v>
       </c>
@@ -2932,10 +2911,10 @@
         <v>2026</v>
       </c>
       <c r="E148">
-        <v>-0.17704032887002619</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+        <v>-0.1770403288700262</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149" s="2">
         <v>45891</v>
       </c>
@@ -2943,16 +2922,16 @@
         <v>2025</v>
       </c>
       <c r="C149">
-        <v>0.10762760044247251</v>
+        <v>0.1076276004424725</v>
       </c>
       <c r="D149">
         <v>2026</v>
       </c>
       <c r="E149">
-        <v>-0.42814445424869119</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+        <v>-0.4281444542486912</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
       <c r="A150" s="2">
         <v>45986</v>
       </c>
@@ -2960,13 +2939,13 @@
         <v>2025</v>
       </c>
       <c r="C150">
-        <v>0.21940175159154141</v>
+        <v>0.2194017515915414</v>
       </c>
       <c r="D150">
         <v>2026</v>
       </c>
       <c r="E150">
-        <v>-0.18831859814396609</v>
+        <v>-0.1883185981439661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>